<commit_message>
add reward logic | adjust Reward_Table
</commit_message>
<xml_diff>
--- a/Slot_Machine/Reward_Table.xlsx
+++ b/Slot_Machine/Reward_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyeonghoon_park/Library/CloudStorage/OneDrive-pnw.edu/2023_Spring/ITS36200/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyeonghoon_park/Online-Casino/Slot_Machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C779D5E-A6E8-6647-8F12-C017B34DEF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBF31F6-0A8D-594C-AB83-0A98C5E3BB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{AF751C95-DA6B-4F47-BFA0-7498995A8105}"/>
+    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="18380" xr2:uid="{AF751C95-DA6B-4F47-BFA0-7498995A8105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t>🍒</t>
   </si>
@@ -71,15 +71,9 @@
     <t>🍒ANYANY</t>
   </si>
   <si>
-    <t>🍋🍋💎</t>
-  </si>
-  <si>
     <t>🍊🍊💎</t>
   </si>
   <si>
-    <t>🍋🍋🍋</t>
-  </si>
-  <si>
     <t>🍇🍇💎</t>
   </si>
   <si>
@@ -90,6 +84,15 @@
   </si>
   <si>
     <t>🍉🍉💎</t>
+  </si>
+  <si>
+    <t>🍈</t>
+  </si>
+  <si>
+    <t>🍈🍈🍈</t>
+  </si>
+  <si>
+    <t>🍈🍈💎</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,10 +469,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E1" s="1">
         <v>1</v>
@@ -483,10 +486,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -512,168 +515,174 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>2000</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1">
         <v>4000</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1">
         <v>6000</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
         <v>2000</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1">
         <v>4000</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1">
         <v>6000</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>2000</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1">
         <v>3000</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.05</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1">
         <v>1000</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>2000</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1">
         <v>3000</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
       <c r="B7">
-        <f>SUM(B1:B6)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1">
+        <v>150</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B1:B7)</f>
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1">
-        <v>85</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1">
-        <v>170</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1">
-        <v>255</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1">
-        <v>255</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>11</v>
+        <v>150</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -681,19 +690,19 @@
         <v>4</v>
       </c>
       <c r="E9" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="1">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>4</v>
@@ -701,25 +710,25 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1">
         <v>60</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1">
-        <v>120</v>
-      </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" s="1">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -727,19 +736,19 @@
         <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="1">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="H11" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="1">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>2</v>
@@ -750,19 +759,19 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>1</v>
@@ -773,19 +782,19 @@
         <v>10</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
line reward_table, reslice the images
</commit_message>
<xml_diff>
--- a/Slot_Machine/Reward_Table.xlsx
+++ b/Slot_Machine/Reward_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyeonghoon_park/Online-Casino/Slot_Machine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyeonghoon_park/Online-Casino/slot_machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E364F0-CCEB-BE42-B809-DB2A977FBC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8513E40F-0C57-3F47-ADA5-CF2AD0FF9D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="18380" xr2:uid="{AF751C95-DA6B-4F47-BFA0-7498995A8105}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="19600" windowHeight="18380" xr2:uid="{AF751C95-DA6B-4F47-BFA0-7498995A8105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,52 +47,52 @@
     <t>🍒🍒🍒</t>
   </si>
   <si>
-    <t>🍊</t>
-  </si>
-  <si>
-    <t>🍊🍊🍊</t>
-  </si>
-  <si>
-    <t>💎</t>
-  </si>
-  <si>
-    <t>💎💎💎</t>
-  </si>
-  <si>
     <t>🍋</t>
   </si>
   <si>
-    <t>🍇</t>
-  </si>
-  <si>
-    <t>🍉</t>
-  </si>
-  <si>
     <t>🍒ANYANY</t>
   </si>
   <si>
-    <t>🍊🍊💎</t>
-  </si>
-  <si>
-    <t>🍇🍇💎</t>
-  </si>
-  <si>
-    <t>🍇🍇🍇</t>
-  </si>
-  <si>
-    <t>🍉🍉🍉</t>
-  </si>
-  <si>
-    <t>🍉🍉💎</t>
-  </si>
-  <si>
-    <t>🍈</t>
-  </si>
-  <si>
-    <t>🍈🍈🍈</t>
-  </si>
-  <si>
-    <t>🍈🍈💎</t>
+    <t>🔔🔔🔔</t>
+  </si>
+  <si>
+    <t>🔔</t>
+  </si>
+  <si>
+    <t>💰💰💰</t>
+  </si>
+  <si>
+    <t>💰💰🔔</t>
+  </si>
+  <si>
+    <t>💰</t>
+  </si>
+  <si>
+    <t>🫐</t>
+  </si>
+  <si>
+    <t>🫐🫐🫐</t>
+  </si>
+  <si>
+    <t>🫐🫐🔔</t>
+  </si>
+  <si>
+    <t>🍀</t>
+  </si>
+  <si>
+    <t>🍀🍀🍀</t>
+  </si>
+  <si>
+    <t>🍀🍀🔔</t>
+  </si>
+  <si>
+    <t>🍎</t>
+  </si>
+  <si>
+    <t>🍎🍎🍎</t>
+  </si>
+  <si>
+    <t>🍎🍎🔔</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +469,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>0.25</v>
@@ -492,112 +492,112 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>10000</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>20000</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1">
         <v>30000</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0.2</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
         <v>2000</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1">
         <v>4000</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I3" s="1">
         <v>6000</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0.15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>2000</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
         <v>4000</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1">
         <v>6000</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1">
         <v>2000</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" s="1">
         <v>3000</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -608,54 +608,54 @@
         <v>0.05</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
         <v>1000</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1">
         <v>2000</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1">
         <v>3000</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1">
         <v>150</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -664,71 +664,71 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1">
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1">
         <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1">
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D9" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1">
         <v>60</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I9" s="1">
         <v>90</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1">
         <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1">
         <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I10" s="1">
         <v>90</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -779,25 +779,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G13" s="1">
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1">
         <v>3</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>